<commit_message>
genereren nieuwe cohorten en cohortjaren
</commit_message>
<xml_diff>
--- a/public/cohort/fileExcel/xlsxUIT/NE PTA en onderwijsprogramma.xlsx
+++ b/public/cohort/fileExcel/xlsxUIT/NE PTA en onderwijsprogramma.xlsx
@@ -1489,7 +1489,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2">
         <v>21</v>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -4200,7 +4200,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -5181,7 +5181,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -5814,12 +5814,12 @@
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="G2" s="36" t="str">
         <f>IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
-        <v>verouderd PTA</v>
+        <v>Dit is het programma van de huidige M2 (cohort 2021 - 2022)</v>
       </c>
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
@@ -5841,21 +5841,25 @@
       <c r="A4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="2"/>
       <c r="G4" s="17" t="str">
         <f>CONCATENATE(B4," leerlaag ",B6,"4 (schooljaar ",B7," - ",B7+1,")")</f>
-        <v> leerlaag 4 (schooljaar  - 1)</v>
+        <v>NE leerlaag M4 (schooljaar 2021 - 2022)</v>
       </c>
     </row>
     <row r="5" spans="1:17" customHeight="1" ht="34.5">
       <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
       <c r="D5" s="7" t="s">
         <v>35</v>
       </c>
@@ -5897,7 +5901,9 @@
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="27" t="s">
@@ -5923,7 +5929,9 @@
       <c r="A7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>2021</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="27" t="s">
@@ -5949,7 +5957,9 @@
       <c r="A8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>181</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="27" t="s">
@@ -5977,7 +5987,7 @@
       </c>
       <c r="B9" s="4">
         <f>IF(B6="A",B7+3,IF(B6="H",B7+2,B7+1))</f>
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -6006,7 +6016,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6073,15 +6083,17 @@
       </c>
       <c r="B13" s="4">
         <f>B7-B11</f>
-        <v>-2020</v>
+        <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>451</v>
+      </c>
       <c r="G13" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G4)</f>
-        <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 4 (schooljaar  - 1)</v>
+        <v>Algemene opmerkingen bij het jaarprogramma van  NE leerlaag M4 (schooljaar 2021 - 2022)</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
@@ -6096,7 +6108,7 @@
       </c>
       <c r="B14" s="7">
         <f>B15+B11-B7</f>
-        <v>2024</v>
+        <v>2</v>
       </c>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
@@ -6112,7 +6124,7 @@
       </c>
       <c r="B15" s="7">
         <f>IF(B6="M",3,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:17" customHeight="1" ht="30.75">
@@ -6122,7 +6134,7 @@
       <c r="D16" s="2"/>
       <c r="G16" s="17" t="str">
         <f>CONCATENATE(B4," leerlaag ",B6,"5 (schooljaar ",B7+1," - ",B7+2,")")</f>
-        <v> leerlaag 5 (schooljaar 1 - 2)</v>
+        <v>NE leerlaag M5 (schooljaar 2022 - 2023)</v>
       </c>
     </row>
     <row r="17" spans="1:17" customHeight="1" ht="34.5">
@@ -6299,10 +6311,12 @@
       <c r="C25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>452</v>
+      </c>
       <c r="G25" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G16)</f>
-        <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 5 (schooljaar 1 - 2)</v>
+        <v>Algemene opmerkingen bij het jaarprogramma van  NE leerlaag M5 (schooljaar 2022 - 2023)</v>
       </c>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -6327,7 +6341,7 @@
       <c r="D28" s="2"/>
       <c r="G28" s="17" t="str">
         <f>CONCATENATE(B4," leerlaag ",B6,"6 (schooljaar ",B7+2," - ",B9,")")</f>
-        <v> leerlaag 6 (schooljaar 2 - 1)</v>
+        <v>NE leerlaag M6 (schooljaar 2023 - 2022)</v>
       </c>
     </row>
     <row r="29" spans="1:17" customHeight="1" ht="34.5">
@@ -6507,7 +6521,7 @@
       <c r="D37" s="2"/>
       <c r="G37" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G28)</f>
-        <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 6 (schooljaar 2 - 1)</v>
+        <v>Algemene opmerkingen bij het jaarprogramma van  NE leerlaag M6 (schooljaar 2023 - 2022)</v>
       </c>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -6581,6 +6595,41 @@
       <formula>ISBLANK($O30)</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="11">
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="G6:G11">
+      <formula1>instellingen!$G$2:$G$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="G30:G35">
+      <formula1>instellingen!$G$2:$G$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="J6:J11">
+      <formula1>instellingen!$H$2:$H$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="J18:J23">
+      <formula1>instellingen!$H$2:$H$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="J30:J35">
+      <formula1>instellingen!$H$2:$H$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="M6:M11">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="M18:M23">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="M30:M35">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="O6:O11">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="O18:O23">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="O30:O35">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
@@ -6831,7 +6880,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7666,7 +7715,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -8396,12 +8445,12 @@
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="G2" s="36" t="str">
         <f>IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
-        <v>verouderd PTA</v>
+        <v>Dit is het programma van de huidige H3 (cohort 2021 - 2023)</v>
       </c>
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
@@ -8423,21 +8472,25 @@
       <c r="A4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="2"/>
       <c r="G4" s="17" t="str">
         <f>CONCATENATE(B4," leerlaag ",B6,"4 (schooljaar ",B7," - ",B7+1,")")</f>
-        <v> leerlaag 4 (schooljaar  - 1)</v>
+        <v>NE leerlaag H4 (schooljaar 2021 - 2022)</v>
       </c>
     </row>
     <row r="5" spans="1:17" customHeight="1" ht="34.5">
       <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
       <c r="D5" s="7" t="s">
         <v>35</v>
       </c>
@@ -8479,7 +8532,9 @@
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="27" t="s">
@@ -8505,7 +8560,9 @@
       <c r="A7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>2021</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="G7" s="27" t="s">
@@ -8531,7 +8588,9 @@
       <c r="A8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>182</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="27" t="s">
@@ -8559,7 +8618,7 @@
       </c>
       <c r="B9" s="4">
         <f>IF(B6="A",B7+3,IF(B6="H",B7+2,B7+1))</f>
-        <v>1</v>
+        <v>2023</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -8588,7 +8647,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -8655,15 +8714,17 @@
       </c>
       <c r="B13" s="4">
         <f>B7-B11</f>
-        <v>-2020</v>
+        <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>453</v>
+      </c>
       <c r="G13" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G4)</f>
-        <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 4 (schooljaar  - 1)</v>
+        <v>Algemene opmerkingen bij het jaarprogramma van  NE leerlaag H4 (schooljaar 2021 - 2022)</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
@@ -8678,7 +8739,7 @@
       </c>
       <c r="B14" s="7">
         <f>B15+B11-B7</f>
-        <v>2024</v>
+        <v>3</v>
       </c>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
@@ -8704,7 +8765,7 @@
       <c r="D16" s="2"/>
       <c r="G16" s="17" t="str">
         <f>CONCATENATE(B4," leerlaag ",B6,"5 (schooljaar ",B7+1," - ",B7+2,")")</f>
-        <v> leerlaag 5 (schooljaar 1 - 2)</v>
+        <v>NE leerlaag H5 (schooljaar 2022 - 2023)</v>
       </c>
     </row>
     <row r="17" spans="1:17" customHeight="1" ht="34.5">
@@ -8881,10 +8942,12 @@
       <c r="C25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>454</v>
+      </c>
       <c r="G25" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G16)</f>
-        <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 5 (schooljaar 1 - 2)</v>
+        <v>Algemene opmerkingen bij het jaarprogramma van  NE leerlaag H5 (schooljaar 2022 - 2023)</v>
       </c>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
@@ -8909,7 +8972,7 @@
       <c r="D28" s="2"/>
       <c r="G28" s="17" t="str">
         <f>CONCATENATE(B4," leerlaag ",B6,"6 (schooljaar ",B7+2," - ",B9,")")</f>
-        <v> leerlaag 6 (schooljaar 2 - 1)</v>
+        <v>NE leerlaag H6 (schooljaar 2023 - 2023)</v>
       </c>
     </row>
     <row r="29" spans="1:17" customHeight="1" ht="34.5">
@@ -9089,7 +9152,7 @@
       <c r="D37" s="2"/>
       <c r="G37" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G28)</f>
-        <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 6 (schooljaar 2 - 1)</v>
+        <v>Algemene opmerkingen bij het jaarprogramma van  NE leerlaag H6 (schooljaar 2023 - 2023)</v>
       </c>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
@@ -9163,6 +9226,44 @@
       <formula>ISBLANK($O30)</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="12">
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="G6:G11">
+      <formula1>instellingen!$G$2:$G$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="G18:G23">
+      <formula1>instellingen!$G$2:$G$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="G30:G35">
+      <formula1>instellingen!$G$2:$G$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="J6:J11">
+      <formula1>instellingen!$H$2:$H$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="J18:J23">
+      <formula1>instellingen!$H$2:$H$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="J30:J35">
+      <formula1>instellingen!$H$2:$H$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="M6:M11">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="M18:M23">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="M30:M35">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="O6:O11">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="O18:O23">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="ongeldige waarde" sqref="O30:O35">
+      <formula1>instellingen!$I$2:$I$4</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
@@ -9463,7 +9564,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2">
         <v>11</v>
@@ -10362,7 +10463,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44340.451041667</v>
+        <v>44340.505590278</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>

</xml_diff>